<commit_message>
0501 modifed bespin PC
</commit_message>
<xml_diff>
--- a/excelread-case1.xlsx
+++ b/excelread-case1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\02_AhaPython\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE1E634-AF5C-46EA-8A99-DF759C28C2D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A79BB23-0694-4B95-805B-5315D53CF042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{D05ACCBB-E9BD-43A9-8DF4-3C2ABB2246C1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D05ACCBB-E9BD-43A9-8DF4-3C2ABB2246C1}"/>
   </bookViews>
   <sheets>
     <sheet name="테이블목록" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>SEQ</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -80,6 +80,42 @@
   </si>
   <si>
     <t>컬럼정의</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dept</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>employee</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>company</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부서</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>직원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회사</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'부서' 속성을 갖는 엔터티</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'직원' 속성을 갖는 엔터티</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'회사' 속성을 갖는 엔터티</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -156,7 +192,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -167,6 +203,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -485,15 +524,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{636D7023-1003-40D9-BF61-01A99A052366}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="11.3984375" customWidth="1"/>
     <col min="3" max="3" width="12.796875" customWidth="1"/>
-    <col min="4" max="4" width="20.09765625" customWidth="1"/>
+    <col min="4" max="4" width="22.296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -511,22 +550,46 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" s="3"/>
@@ -562,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1AE5CC9-5E3D-46CF-B326-AA30E492F53C}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>

</xml_diff>